<commit_message>
moved some folders around so that I2C comes first
</commit_message>
<xml_diff>
--- a/Microprocessor Prototyping 180.xlsx
+++ b/Microprocessor Prototyping 180.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">Microprocessor Prototyping 180</t>
   </si>
@@ -134,6 +134,9 @@
     <t xml:space="preserve">Going Further: Telemetry Recorder</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.adafruit.com/products/2652</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arduino Uno</t>
   </si>
   <si>
@@ -161,10 +164,10 @@
     <t xml:space="preserve">LED Array</t>
   </si>
   <si>
-    <t xml:space="preserve">Touch Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLED Display</t>
+    <t xml:space="preserve">Pressure/Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLED</t>
   </si>
   <si>
     <t xml:space="preserve">9DOF</t>
@@ -629,9 +632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1676160</xdr:colOff>
+      <xdr:colOff>1675800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1228320</xdr:rowOff>
+      <xdr:rowOff>1227960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,7 +648,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="38160" y="0"/>
-          <a:ext cx="1638000" cy="1228320"/>
+          <a:ext cx="1637640" cy="1227960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -662,11 +665,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>76320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1685520</xdr:colOff>
+      <xdr:colOff>1685160</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1238040</xdr:rowOff>
     </xdr:to>
@@ -681,8 +684,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76320" y="1323720"/>
-          <a:ext cx="1609200" cy="1218960"/>
+          <a:off x="76320" y="1324080"/>
+          <a:ext cx="1608840" cy="1218600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -703,9 +706,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1723680</xdr:colOff>
+      <xdr:colOff>1723320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1276200</xdr:rowOff>
+      <xdr:rowOff>1275840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -719,7 +722,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="2657520"/>
-          <a:ext cx="1647360" cy="1238040"/>
+          <a:ext cx="1647000" cy="1237680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,9 +743,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1609200</xdr:colOff>
+      <xdr:colOff>1608840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1399680</xdr:rowOff>
+      <xdr:rowOff>1399320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -756,7 +759,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="228600" y="4076640"/>
-          <a:ext cx="1380600" cy="1380600"/>
+          <a:ext cx="1380240" cy="1380240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,9 +780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1409400</xdr:colOff>
+      <xdr:colOff>1409040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1161720</xdr:rowOff>
+      <xdr:rowOff>1161360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -793,7 +796,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="285840" y="5572080"/>
-          <a:ext cx="1123560" cy="1123560"/>
+          <a:ext cx="1123200" cy="1123200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -814,9 +817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1342800</xdr:colOff>
+      <xdr:colOff>1342440</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1076040</xdr:rowOff>
+      <xdr:rowOff>1075680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -830,7 +833,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="304920" y="6838920"/>
-          <a:ext cx="1037880" cy="1037880"/>
+          <a:ext cx="1037520" cy="1037520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,11 +850,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>304920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1380960</xdr:colOff>
+      <xdr:colOff>1380600</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>1123560</xdr:rowOff>
     </xdr:to>
@@ -866,8 +869,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304920" y="8019720"/>
-          <a:ext cx="1076040" cy="1076040"/>
+          <a:off x="304920" y="8020080"/>
+          <a:ext cx="1075680" cy="1075680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -888,9 +891,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1676160</xdr:colOff>
+      <xdr:colOff>1675800</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1199520</xdr:rowOff>
+      <xdr:rowOff>1199160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -904,7 +907,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="9239040"/>
-          <a:ext cx="1599840" cy="1190160"/>
+          <a:ext cx="1599480" cy="1189800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -921,11 +924,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>314280</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1361520</xdr:colOff>
+      <xdr:colOff>1361160</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>1094760</xdr:rowOff>
     </xdr:to>
@@ -940,8 +943,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314280" y="10639080"/>
-          <a:ext cx="1047240" cy="1047240"/>
+          <a:off x="314280" y="10639440"/>
+          <a:ext cx="1046880" cy="1046880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -956,19 +959,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:colOff>76320</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1618920</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1161360</xdr:rowOff>
+      <xdr:colOff>1713960</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1266120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="image03.jpg" descr=""/>
+        <xdr:cNvPr id="9" name="image10.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -977,8 +980,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="85680" y="11763000"/>
-          <a:ext cx="1533240" cy="1152000"/>
+          <a:off x="76320" y="13154040"/>
+          <a:ext cx="1637640" cy="1227960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,19 +996,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1714320</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1266480</xdr:rowOff>
+      <xdr:colOff>1599480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1599480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="image10.jpg" descr=""/>
+        <xdr:cNvPr id="10" name="image09.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1014,8 +1017,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76320" y="13154040"/>
-          <a:ext cx="1638000" cy="1228320"/>
+          <a:off x="152280" y="14792040"/>
+          <a:ext cx="1447200" cy="1447200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1030,19 +1033,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152280</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:colOff>171360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1599840</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1599840</xdr:rowOff>
+      <xdr:colOff>1618560</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1485360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="image09.jpg" descr=""/>
+        <xdr:cNvPr id="11" name="image11.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1051,8 +1054,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="152280" y="14792040"/>
-          <a:ext cx="1447560" cy="1447560"/>
+          <a:off x="171360" y="16497360"/>
+          <a:ext cx="1447200" cy="1447200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1067,19 +1070,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171360</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:colOff>76320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1618920</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1485720</xdr:rowOff>
+      <xdr:colOff>1752120</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1685160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="image11.jpg" descr=""/>
+        <xdr:cNvPr id="12" name="image12.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1088,8 +1091,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171360" y="16497360"/>
-          <a:ext cx="1447560" cy="1447560"/>
+          <a:off x="76320" y="18173520"/>
+          <a:ext cx="1675800" cy="1675800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1101,22 +1104,22 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:colOff>180000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1752480</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1685520</xdr:rowOff>
+      <xdr:colOff>1664640</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1195200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="image12.jpg" descr=""/>
+        <xdr:cNvPr id="13" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1125,8 +1128,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76320" y="18173520"/>
-          <a:ext cx="1676160" cy="1676160"/>
+          <a:off x="180000" y="11887560"/>
+          <a:ext cx="1484640" cy="1061280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1148,16 +1151,17 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1610,22 +1614,26 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3418367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="B1" s="38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/50","https://www.adafruit.com/products/50")</f>
@@ -1638,7 +1646,7 @@
     <row r="2" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/62","https://www.adafruit.com/products/62")</f>
@@ -1651,7 +1659,7 @@
     <row r="3" customFormat="false" ht="113.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/239","https://www.adafruit.com/products/239")</f>
@@ -1664,7 +1672,7 @@
     <row r="4" customFormat="false" ht="116.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/12062","https://www.sparkfun.com/products/12062")</f>
@@ -1677,7 +1685,7 @@
     <row r="5" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/11507","https://www.sparkfun.com/products/11507")</f>
@@ -1690,7 +1698,7 @@
     <row r="6" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/11367","https://www.sparkfun.com/products/11367")</f>
@@ -1703,7 +1711,7 @@
     <row r="7" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/12630","https://www.sparkfun.com/products/12630")</f>
@@ -1716,7 +1724,7 @@
     <row r="8" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/1384","https://www.adafruit.com/products/1384")</f>
@@ -1729,7 +1737,7 @@
     <row r="9" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13795","https://www.sparkfun.com/products/13795")</f>
@@ -1742,20 +1750,19 @@
     <row r="10" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="39" t="str">
-        <f aca="false">HYPERLINK("https://www.adafruit.com/products/1602","https://www.adafruit.com/products/1602")</f>
-        <v>https://www.adafruit.com/products/1602</v>
+        <v>47</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>37</v>
       </c>
       <c r="D10" s="41" t="n">
-        <v>7.95</v>
+        <v>19.95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/931","https://www.adafruit.com/products/931")</f>
@@ -1768,7 +1775,7 @@
     <row r="12" customFormat="false" ht="143.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13944","https://www.sparkfun.com/products/13944")</f>
@@ -1781,7 +1788,7 @@
     <row r="13" customFormat="false" ht="134.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/544","https://www.sparkfun.com/products/544")</f>
@@ -1794,7 +1801,7 @@
     <row r="14" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13833","https://www.sparkfun.com/products/13833")</f>
@@ -1810,20 +1817,20 @@
       <c r="C15" s="42"/>
       <c r="D15" s="41"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="38"/>
       <c r="C16" s="43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="44" t="str">
+      <c r="C17" s="44" t="n">
         <f aca="false">SUM(D1:D14)</f>
-        <v>135.85</v>
+        <v>147.85</v>
       </c>
       <c r="D17" s="41"/>
     </row>

</xml_diff>

<commit_message>
broke out the parts list to a seperate document
</commit_message>
<xml_diff>
--- a/Microprocessor Prototyping 180.xlsx
+++ b/Microprocessor Prototyping 180.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Microprocessor Prototyping 180</t>
   </si>
@@ -131,39 +131,42 @@
     <t xml:space="preserve">Going Further: Data Logger</t>
   </si>
   <si>
+    <t xml:space="preserve">Arduino Uno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hookup Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strippers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-segment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sparkfun.com/products/11408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure/Temp</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.adafruit.com/products/2652</t>
   </si>
   <si>
-    <t xml:space="preserve">Arduino Uno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arduino USB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breadboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEDs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hookup Wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strippers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure/Temp</t>
-  </si>
-  <si>
     <t xml:space="preserve">OLED</t>
   </si>
   <si>
@@ -174,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">SD Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/SanDisk-MicroSD-TransFlash-Adapter-camcorder/dp/B000VOU91U/ref=sr_1_19?s=wireless&amp;ie=UTF8&amp;qid=1492139570&amp;sr=1-19&amp;keywords=SD+card+micro+adapter&amp;refinements=p_36%3A2491155011</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL:</t>
@@ -629,9 +635,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1675440</xdr:colOff>
+      <xdr:colOff>1675080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1227600</xdr:rowOff>
+      <xdr:rowOff>1227240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,7 +651,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="38160" y="0"/>
-          <a:ext cx="1637280" cy="1227600"/>
+          <a:ext cx="1636920" cy="1227240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -662,11 +668,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>76320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1684800</xdr:colOff>
+      <xdr:colOff>1684440</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1237680</xdr:rowOff>
     </xdr:to>
@@ -681,8 +687,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76320" y="1324080"/>
-          <a:ext cx="1608480" cy="1218240"/>
+          <a:off x="76320" y="1324440"/>
+          <a:ext cx="1608120" cy="1217880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -703,9 +709,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1722960</xdr:colOff>
+      <xdr:colOff>1722600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1275480</xdr:rowOff>
+      <xdr:rowOff>1275120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -719,7 +725,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="2657520"/>
-          <a:ext cx="1646640" cy="1237320"/>
+          <a:ext cx="1646280" cy="1236960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,9 +746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1608480</xdr:colOff>
+      <xdr:colOff>1608120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1398960</xdr:rowOff>
+      <xdr:rowOff>1398600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -756,7 +762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="228600" y="4076640"/>
-          <a:ext cx="1379880" cy="1379880"/>
+          <a:ext cx="1379520" cy="1379520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,9 +783,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1408680</xdr:colOff>
+      <xdr:colOff>1408320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1161000</xdr:rowOff>
+      <xdr:rowOff>1160640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -793,7 +799,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="285840" y="5572080"/>
-          <a:ext cx="1122840" cy="1122840"/>
+          <a:ext cx="1122480" cy="1122480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -814,9 +820,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1342080</xdr:colOff>
+      <xdr:colOff>1341720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1075320</xdr:rowOff>
+      <xdr:rowOff>1074960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -830,7 +836,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="304920" y="6838920"/>
-          <a:ext cx="1037160" cy="1037160"/>
+          <a:ext cx="1036800" cy="1036800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,11 +853,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>304920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1380240</xdr:colOff>
+      <xdr:colOff>1379880</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>1123200</xdr:rowOff>
     </xdr:to>
@@ -866,8 +872,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304920" y="8020080"/>
-          <a:ext cx="1075320" cy="1075320"/>
+          <a:off x="304920" y="8020440"/>
+          <a:ext cx="1074960" cy="1074960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -888,9 +894,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1675440</xdr:colOff>
+      <xdr:colOff>1675080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1198800</xdr:rowOff>
+      <xdr:rowOff>1198440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -904,7 +910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="9239040"/>
-          <a:ext cx="1599120" cy="1189440"/>
+          <a:ext cx="1598760" cy="1189080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -919,19 +925,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>314280</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:colOff>76320</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1360800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1094400</xdr:rowOff>
+      <xdr:colOff>1713240</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1265400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="image00.jpg" descr=""/>
+        <xdr:cNvPr id="8" name="image10.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -940,8 +946,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314280" y="10639440"/>
-          <a:ext cx="1046520" cy="1046520"/>
+          <a:off x="76320" y="13154040"/>
+          <a:ext cx="1636920" cy="1227240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -956,19 +962,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1713600</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1265760</xdr:rowOff>
+      <xdr:colOff>1598760</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1598760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="image10.jpg" descr=""/>
+        <xdr:cNvPr id="9" name="image09.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -977,8 +983,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76320" y="13154040"/>
-          <a:ext cx="1637280" cy="1227600"/>
+          <a:off x="152280" y="14792040"/>
+          <a:ext cx="1446480" cy="1446480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,19 +999,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152280</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:colOff>171360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1599120</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1599120</xdr:rowOff>
+      <xdr:colOff>1617840</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1484640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="image09.jpg" descr=""/>
+        <xdr:cNvPr id="10" name="image11.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1014,82 +1020,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="152280" y="14792040"/>
-          <a:ext cx="1446840" cy="1446840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>171360</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1618200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1485000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="image11.jpg" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="171360" y="16497360"/>
-          <a:ext cx="1446840" cy="1446840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1751760</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1684800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="image12.jpg" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="76320" y="18173520"/>
-          <a:ext cx="1675440" cy="1675440"/>
+          <a:ext cx="1446480" cy="1446480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1110,13 +1042,87 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1664280</xdr:colOff>
+      <xdr:colOff>1663920</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1194840</xdr:rowOff>
+      <xdr:rowOff>1194480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 1" descr=""/>
+        <xdr:cNvPr id="11" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180000" y="11887560"/>
+          <a:ext cx="1483920" cy="1060560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>270360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>52200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1422360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1147680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="270360" y="10643760"/>
+          <a:ext cx="1152000" cy="1095480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>100080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>236520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1572480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1636920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1125,8 +1131,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="180000" y="11887560"/>
-          <a:ext cx="1484280" cy="1060920"/>
+          <a:off x="100080" y="18400680"/>
+          <a:ext cx="1472400" cy="1400400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1148,17 +1154,17 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="A8:D17 J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4132653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1598,26 +1604,24 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="38" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/50","https://www.adafruit.com/products/50")</f>
@@ -1630,7 +1634,7 @@
     <row r="2" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/62","https://www.adafruit.com/products/62")</f>
@@ -1643,7 +1647,7 @@
     <row r="3" customFormat="false" ht="113.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/239","https://www.adafruit.com/products/239")</f>
@@ -1656,7 +1660,7 @@
     <row r="4" customFormat="false" ht="116.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/12062","https://www.sparkfun.com/products/12062")</f>
@@ -1669,7 +1673,7 @@
     <row r="5" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/11507","https://www.sparkfun.com/products/11507")</f>
@@ -1682,7 +1686,7 @@
     <row r="6" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/11367","https://www.sparkfun.com/products/11367")</f>
@@ -1695,7 +1699,7 @@
     <row r="7" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/12630","https://www.sparkfun.com/products/12630")</f>
@@ -1708,7 +1712,7 @@
     <row r="8" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/1384","https://www.adafruit.com/products/1384")</f>
@@ -1721,14 +1725,13 @@
     <row r="9" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="39" t="str">
-        <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13795","https://www.sparkfun.com/products/13795")</f>
-        <v>https://www.sparkfun.com/products/13795</v>
-      </c>
       <c r="D9" s="41" t="n">
-        <v>8.95</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1737,7 +1740,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D10" s="41" t="n">
         <v>19.95</v>
@@ -1746,7 +1749,7 @@
     <row r="11" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.adafruit.com/products/931","https://www.adafruit.com/products/931")</f>
@@ -1759,7 +1762,7 @@
     <row r="12" customFormat="false" ht="143.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13944","https://www.sparkfun.com/products/13944")</f>
@@ -1772,7 +1775,7 @@
     <row r="13" customFormat="false" ht="134.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="39" t="str">
         <f aca="false">HYPERLINK("https://www.sparkfun.com/products/544","https://www.sparkfun.com/products/544")</f>
@@ -1785,14 +1788,13 @@
     <row r="14" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="39" t="str">
-        <f aca="false">HYPERLINK("https://www.sparkfun.com/products/13833","https://www.sparkfun.com/products/13833")</f>
-        <v>https://www.sparkfun.com/products/13833</v>
+        <v>51</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>52</v>
       </c>
       <c r="D14" s="41" t="n">
-        <v>12.95</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1805,7 +1807,7 @@
       <c r="A16" s="4"/>
       <c r="B16" s="38"/>
       <c r="C16" s="43" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16" s="44"/>
     </row>
@@ -1814,7 +1816,7 @@
       <c r="B17" s="38"/>
       <c r="C17" s="44" t="n">
         <f aca="false">SUM(D1:D14)</f>
-        <v>147.85</v>
+        <v>135.89</v>
       </c>
       <c r="D17" s="41"/>
     </row>

</xml_diff>